<commit_message>
Se agrego el planeta en el registro planetario
</commit_message>
<xml_diff>
--- a/Rubrica Laboratorio 3.xlsx
+++ b/Rubrica Laboratorio 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darinka\Desktop\SISTEMAS DISTRIBUIDOS\3. Tareas\Tarea3\codigo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0011593C-9C5B-4895-8AEA-CA48CA4EF43E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B202E8-9D10-4B72-96A9-55943E3B1EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A4744F64-40AA-46F3-A2F3-6961712D08D4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="131">
   <si>
     <t>Puntaje obtenido</t>
   </si>
@@ -973,6 +973,9 @@
   </si>
   <si>
     <t>Total actual -&gt;</t>
+  </si>
+  <si>
+    <t>Acumulado</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1100,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1205,12 +1208,149 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1238,9 +1378,6 @@
     </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1281,9 +1418,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1311,8 +1445,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1320,73 +1469,94 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1707,131 +1877,139 @@
   <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="76" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="76" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.28515625" style="8" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" style="8" customWidth="1"/>
     <col min="4" max="4" width="9" style="8" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" style="33"/>
-    <col min="7" max="16384" width="11.5703125" style="11"/>
+    <col min="6" max="6" width="11.5703125" style="31"/>
+    <col min="7" max="16384" width="11.5703125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="34"/>
+      <c r="E1" s="45" t="s">
         <v>128</v>
       </c>
+      <c r="F1" s="45" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="51">
+      <c r="B2" s="47"/>
+      <c r="C2" s="48">
         <v>4</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="53">
+      <c r="D2" s="49"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="51">
         <f>SUM(E3:E4)</f>
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="52" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45">
+      <c r="B3" s="32"/>
+      <c r="C3" s="32">
         <v>2</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="E3" s="47">
+      <c r="E3" s="33">
         <f>IF(D3="ok",C3,0)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="F3" s="53"/>
+    </row>
+    <row r="4" spans="1:6" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="54" t="s">
         <v>126</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45">
+      <c r="B4" s="55"/>
+      <c r="C4" s="55">
         <v>2</v>
       </c>
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="E4" s="47">
+      <c r="E4" s="56">
         <f t="shared" ref="E4:E35" si="0">IF(D4="ok",C4,0)</f>
         <v>2</v>
       </c>
+      <c r="F4" s="57"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51">
+      <c r="B5" s="47"/>
+      <c r="C5" s="48">
         <v>16</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="53">
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="51">
         <f>SUM(E6:E11)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="46" t="s">
+      <c r="A6" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47">
+      <c r="B6" s="33"/>
+      <c r="C6" s="33">
         <v>3</v>
       </c>
-      <c r="D6" s="47" t="s">
+      <c r="D6" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="E6" s="47">
+      <c r="E6" s="33">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
+      <c r="F6" s="53"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="46" t="s">
+      <c r="A7" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47">
+      <c r="B7" s="33"/>
+      <c r="C7" s="33">
         <v>2</v>
       </c>
-      <c r="D7" s="47" t="s">
+      <c r="D7" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="E7" s="47">
+      <c r="E7" s="33">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="F7" s="53"/>
     </row>
     <row r="8" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="59" t="s">
         <v>109</v>
       </c>
       <c r="B8" s="7"/>
@@ -1843,9 +2021,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F8" s="53"/>
     </row>
     <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="59" t="s">
         <v>110</v>
       </c>
       <c r="B9" s="7"/>
@@ -1857,54 +2036,59 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F9" s="53"/>
     </row>
     <row r="10" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47">
+      <c r="B10" s="33"/>
+      <c r="C10" s="33">
         <v>2</v>
       </c>
-      <c r="D10" s="47" t="s">
+      <c r="D10" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="E10" s="47">
+      <c r="E10" s="33">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="58" t="s">
+      <c r="F10" s="53"/>
+    </row>
+    <row r="11" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="59"/>
-      <c r="C11" s="59">
+      <c r="B11" s="56"/>
+      <c r="C11" s="56">
         <v>2</v>
       </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59">
+      <c r="D11" s="56" t="s">
+        <v>108</v>
+      </c>
+      <c r="E11" s="56">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F11" s="57"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
+      <c r="A12" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="51">
+      <c r="B12" s="47"/>
+      <c r="C12" s="48">
         <v>22</v>
       </c>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="53">
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="51">
         <f>SUM(E13:E17)</f>
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="59" t="s">
         <v>112</v>
       </c>
       <c r="B13" s="7"/>
@@ -1916,25 +2100,27 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F13" s="53"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="48" t="s">
+      <c r="A14" s="60" t="s">
         <v>113</v>
       </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47">
+      <c r="B14" s="33"/>
+      <c r="C14" s="33">
         <v>2</v>
       </c>
-      <c r="D14" s="47" t="s">
+      <c r="D14" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="E14" s="47">
+      <c r="E14" s="33">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="F14" s="53"/>
     </row>
     <row r="15" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="59" t="s">
         <v>114</v>
       </c>
       <c r="B15" s="7"/>
@@ -1946,56 +2132,59 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F15" s="53"/>
     </row>
     <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="60" t="s">
         <v>115</v>
       </c>
-      <c r="B16" s="47"/>
-      <c r="C16" s="47">
+      <c r="B16" s="33"/>
+      <c r="C16" s="33">
         <v>8</v>
       </c>
-      <c r="D16" s="47" t="s">
+      <c r="D16" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="E16" s="47">
+      <c r="E16" s="33">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="48" t="s">
+      <c r="F16" s="53"/>
+    </row>
+    <row r="17" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="61" t="s">
         <v>116</v>
       </c>
-      <c r="B17" s="47"/>
-      <c r="C17" s="47">
+      <c r="B17" s="56"/>
+      <c r="C17" s="56">
         <v>2</v>
       </c>
-      <c r="D17" s="47" t="s">
+      <c r="D17" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="47">
+      <c r="E17" s="56">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="F17" s="57"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="49" t="s">
+      <c r="A18" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="50"/>
-      <c r="C18" s="51">
+      <c r="B18" s="47"/>
+      <c r="C18" s="48">
         <v>14</v>
       </c>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="53">
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="51">
         <f>SUM(E19:E24)</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="59" t="s">
         <v>117</v>
       </c>
       <c r="B19" s="7"/>
@@ -2007,9 +2196,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F19" s="53"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+      <c r="A20" s="59" t="s">
         <v>118</v>
       </c>
       <c r="B20" s="7"/>
@@ -2021,9 +2211,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F20" s="53"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="59" t="s">
         <v>119</v>
       </c>
       <c r="B21" s="7"/>
@@ -2035,9 +2226,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F21" s="53"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="59" t="s">
         <v>120</v>
       </c>
       <c r="B22" s="7"/>
@@ -2049,9 +2241,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F22" s="53"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="59" t="s">
         <v>121</v>
       </c>
       <c r="B23" s="7"/>
@@ -2063,133 +2256,140 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="34" t="s">
+      <c r="F23" s="53"/>
+    </row>
+    <row r="24" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7">
+      <c r="B24" s="63"/>
+      <c r="C24" s="63">
         <v>2</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7">
+      <c r="D24" s="63"/>
+      <c r="E24" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F24" s="57"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="49" t="s">
+      <c r="A25" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="50"/>
-      <c r="C25" s="51">
+      <c r="B25" s="47"/>
+      <c r="C25" s="48">
         <v>12</v>
       </c>
-      <c r="D25" s="53"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="53">
+      <c r="D25" s="49"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="51">
         <f>SUM(E26:E30)</f>
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="48" t="s">
+      <c r="A26" s="60" t="s">
         <v>117</v>
       </c>
-      <c r="B26" s="47"/>
-      <c r="C26" s="47">
+      <c r="B26" s="33"/>
+      <c r="C26" s="33">
         <v>2</v>
       </c>
-      <c r="D26" s="47" t="s">
+      <c r="D26" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="E26" s="47">
+      <c r="E26" s="33">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="F26" s="53"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="48" t="s">
+      <c r="A27" s="60" t="s">
         <v>118</v>
       </c>
-      <c r="B27" s="47"/>
-      <c r="C27" s="47">
+      <c r="B27" s="33"/>
+      <c r="C27" s="33">
         <v>4</v>
       </c>
-      <c r="D27" s="47" t="s">
+      <c r="D27" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="E27" s="47">
+      <c r="E27" s="33">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
+      <c r="F27" s="53"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="48" t="s">
+      <c r="A28" s="60" t="s">
         <v>123</v>
       </c>
-      <c r="B28" s="47"/>
-      <c r="C28" s="47">
+      <c r="B28" s="33"/>
+      <c r="C28" s="33">
         <v>2</v>
       </c>
-      <c r="D28" s="47" t="s">
+      <c r="D28" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="E28" s="47">
+      <c r="E28" s="33">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="F28" s="53"/>
     </row>
     <row r="29" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="60" t="s">
         <v>124</v>
       </c>
-      <c r="B29" s="47"/>
-      <c r="C29" s="47">
+      <c r="B29" s="33"/>
+      <c r="C29" s="33">
         <v>2</v>
       </c>
-      <c r="D29" s="47" t="s">
+      <c r="D29" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="E29" s="47">
+      <c r="E29" s="33">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="46" t="s">
+      <c r="F29" s="53"/>
+    </row>
+    <row r="30" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="64" t="s">
         <v>92</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47">
+      <c r="B30" s="56"/>
+      <c r="C30" s="56">
         <v>2</v>
       </c>
-      <c r="D30" s="47" t="s">
+      <c r="D30" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="E30" s="47">
+      <c r="E30" s="56">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="F30" s="57"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="49" t="s">
+      <c r="A31" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="50"/>
-      <c r="C31" s="51">
+      <c r="B31" s="47"/>
+      <c r="C31" s="48">
         <v>32</v>
       </c>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="53">
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="51">
         <f>SUM(E32:E35)</f>
         <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
+      <c r="A32" s="65" t="s">
         <v>42</v>
       </c>
       <c r="B32" s="7"/>
@@ -2201,25 +2401,27 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F32" s="53"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="46" t="s">
+      <c r="A33" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="47"/>
-      <c r="C33" s="47">
+      <c r="B33" s="33"/>
+      <c r="C33" s="33">
         <v>10</v>
       </c>
-      <c r="D33" s="47" t="s">
+      <c r="D33" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="E33" s="47">
+      <c r="E33" s="33">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="F33" s="53"/>
     </row>
     <row r="34" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="59" t="s">
         <v>125</v>
       </c>
       <c r="B34" s="7"/>
@@ -2231,31 +2433,33 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="24" t="s">
+      <c r="F34" s="53"/>
+    </row>
+    <row r="35" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7">
+      <c r="B35" s="63"/>
+      <c r="C35" s="63">
         <v>4</v>
       </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="54">
+      <c r="D35" s="63"/>
+      <c r="E35" s="63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="55" t="s">
+      <c r="F35" s="57"/>
+    </row>
+    <row r="36" spans="1:6" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="67" t="s">
         <v>129</v>
       </c>
-      <c r="D36" s="56"/>
-      <c r="E36" s="57">
+      <c r="D36" s="68"/>
+      <c r="E36" s="69">
         <f>SUM(E2:E35)</f>
-        <v>45</v>
-      </c>
-      <c r="F36" s="11"/>
+        <v>47</v>
+      </c>
+      <c r="F36" s="10"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
@@ -2272,7 +2476,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B41" s="5" t="s">
@@ -2280,7 +2484,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B42" s="7">
@@ -2288,13 +2492,13 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="12" t="s">
         <v>107</v>
       </c>
       <c r="B43" s="7"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B44" s="7">
@@ -2302,7 +2506,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B45" s="7">
@@ -2310,7 +2514,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="14" t="s">
+      <c r="A46" s="13" t="s">
         <v>11</v>
       </c>
       <c r="B46" s="9">
@@ -2319,7 +2523,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B48" s="9">
@@ -2356,635 +2560,635 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="36">
+      <c r="B2" s="39">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="36">
+      <c r="C2" s="41"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="39">
         <v>2</v>
       </c>
-      <c r="F2" s="37"/>
-      <c r="G2" s="38"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="40"/>
     </row>
     <row r="3" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="39" t="s">
+      <c r="C3" s="42"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="41"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="36"/>
     </row>
     <row r="4" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="39" t="s">
+      <c r="C4" s="42"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="G4" s="41"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="36"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="20">
         <v>0</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="20">
         <v>1</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="20">
         <v>2</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="20">
         <v>3</v>
       </c>
-      <c r="F5" s="42">
+      <c r="F5" s="43">
         <v>5</v>
       </c>
-      <c r="G5" s="42"/>
-    </row>
-    <row r="6" spans="1:7" s="11" customFormat="1" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="G5" s="43"/>
+    </row>
+    <row r="6" spans="1:7" s="10" customFormat="1" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="27" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="11" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+    <row r="7" spans="1:7" s="10" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="19"/>
-    </row>
-    <row r="8" spans="1:7" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="E7" s="18"/>
+    </row>
+    <row r="8" spans="1:7" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="43" t="s">
+      <c r="F8" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="43"/>
-    </row>
-    <row r="9" spans="1:7" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="G8" s="37"/>
+    </row>
+    <row r="9" spans="1:7" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="19"/>
-    </row>
-    <row r="10" spans="1:7" s="11" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="s">
+      <c r="E9" s="18"/>
+    </row>
+    <row r="10" spans="1:7" s="10" customFormat="1" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="19" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="30" t="s">
+    <row r="11" spans="1:7" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="19"/>
+      <c r="E11" s="18"/>
     </row>
     <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="20">
         <v>0</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="20">
         <v>1</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="20">
         <v>2</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="20">
         <v>3</v>
       </c>
-      <c r="F12" s="42">
+      <c r="F12" s="43">
         <v>8</v>
       </c>
-      <c r="G12" s="42"/>
-    </row>
-    <row r="13" spans="1:7" s="11" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="G12" s="43"/>
+    </row>
+    <row r="13" spans="1:7" s="10" customFormat="1" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-    </row>
-    <row r="14" spans="1:7" s="11" customFormat="1" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="1:7" s="10" customFormat="1" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-    </row>
-    <row r="15" spans="1:7" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="E14" s="18"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+    </row>
+    <row r="15" spans="1:7" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="43" t="s">
+      <c r="F15" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="G15" s="43"/>
-    </row>
-    <row r="16" spans="1:7" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+      <c r="G15" s="37"/>
+    </row>
+    <row r="16" spans="1:7" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="43" t="s">
+      <c r="F16" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="G16" s="43"/>
-    </row>
-    <row r="17" spans="1:9" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="G16" s="37"/>
+    </row>
+    <row r="17" spans="1:9" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="27" t="s">
+      <c r="D17" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
       <c r="I17"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="21">
+      <c r="B18" s="20">
         <v>0</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C18" s="20">
         <v>1</v>
       </c>
-      <c r="D18" s="42">
+      <c r="D18" s="43">
         <v>2</v>
       </c>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42">
+      <c r="E18" s="43"/>
+      <c r="F18" s="43">
         <v>3</v>
       </c>
-      <c r="G18" s="42"/>
-      <c r="I18" s="11"/>
+      <c r="G18" s="43"/>
+      <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+      <c r="A19" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="35"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="I19" s="11"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" ht="40.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+      <c r="A20" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="43"/>
-      <c r="F20" s="39" t="s">
+      <c r="E20" s="37"/>
+      <c r="F20" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="G20" s="41"/>
-      <c r="I20" s="11"/>
+      <c r="G20" s="36"/>
+      <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="43" t="s">
+      <c r="D21" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="43"/>
-      <c r="F21" s="39" t="s">
+      <c r="E21" s="37"/>
+      <c r="F21" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="G21" s="41"/>
+      <c r="G21" s="36"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="39" t="s">
+      <c r="D22" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="E22" s="41"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="I22" s="11"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
+      <c r="A23" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="39" t="s">
+      <c r="D23" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="E23" s="41"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="I23" s="11"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="I23" s="10"/>
     </row>
     <row r="24" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="39" t="s">
+      <c r="D24" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="41"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="I24" s="11"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="21">
+      <c r="B25" s="20">
         <v>0</v>
       </c>
-      <c r="C25" s="21">
+      <c r="C25" s="20">
         <v>1</v>
       </c>
-      <c r="D25" s="36">
+      <c r="D25" s="39">
         <v>2</v>
       </c>
-      <c r="E25" s="38"/>
-      <c r="F25" s="36">
+      <c r="E25" s="40"/>
+      <c r="F25" s="39">
         <v>4</v>
       </c>
-      <c r="G25" s="38"/>
+      <c r="G25" s="40"/>
     </row>
     <row r="26" spans="1:9" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="35"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
     </row>
     <row r="27" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
+      <c r="A27" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="43" t="s">
+      <c r="D27" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43" t="s">
+      <c r="E27" s="37"/>
+      <c r="F27" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="G27" s="43"/>
+      <c r="G27" s="37"/>
     </row>
     <row r="28" spans="1:9" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="C28" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="39" t="s">
+      <c r="D28" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="E28" s="41"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="1:9" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
+      <c r="A29" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C29" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="39" t="s">
+      <c r="D29" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="E29" s="41"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
     </row>
     <row r="30" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="43" t="s">
+      <c r="D30" s="37" t="s">
         <v>91</v>
       </c>
-      <c r="E30" s="43"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="21">
+      <c r="B31" s="20">
         <v>0</v>
       </c>
-      <c r="C31" s="21">
+      <c r="C31" s="20">
         <v>1</v>
       </c>
-      <c r="D31" s="21">
+      <c r="D31" s="20">
         <v>4</v>
       </c>
-      <c r="E31" s="21">
+      <c r="E31" s="20">
         <v>6</v>
       </c>
-      <c r="F31" s="21">
+      <c r="F31" s="20">
         <v>10</v>
       </c>
-      <c r="G31" s="21">
+      <c r="G31" s="20">
         <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C32" s="20" t="s">
+      <c r="C32" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="D32" s="20" t="s">
+      <c r="D32" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="E32" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="F32" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="G32" s="20" t="s">
+      <c r="G32" s="19" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="D33" s="20" t="s">
+      <c r="D33" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="E33" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="F33" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="G33" s="23"/>
+      <c r="G33" s="22"/>
     </row>
     <row r="34" spans="1:7" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="20" t="s">
+      <c r="D34" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="E34" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
     </row>
     <row r="35" spans="1:7" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B35" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="D35" s="20" t="s">
+      <c r="D35" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" s="4"/>
@@ -10716,6 +10920,21 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F16:G16"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
     <mergeCell ref="D30:E30"/>
@@ -10731,21 +10950,6 @@
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F16:G16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>